<commit_message>
updated the xlsx file
</commit_message>
<xml_diff>
--- a/Horizontal_bruteforce/fib_pascal _horizontal.xlsx
+++ b/Horizontal_bruteforce/fib_pascal _horizontal.xlsx
@@ -28,19 +28,19 @@
     <t>first_time 0+-</t>
   </si>
   <si>
-    <t>0-+</t>
-  </si>
-  <si>
-    <t>"+0-</t>
-  </si>
-  <si>
-    <t>"+-0</t>
-  </si>
-  <si>
-    <t>-0+</t>
-  </si>
-  <si>
-    <t>-+0</t>
+    <t>first_time 0-+</t>
+  </si>
+  <si>
+    <t>first_time +0-</t>
+  </si>
+  <si>
+    <t>first_time +-0</t>
+  </si>
+  <si>
+    <t>first_time -0+</t>
+  </si>
+  <si>
+    <t>first_time -+0</t>
   </si>
   <si>
     <t>most 0 in -0+</t>

</xml_diff>